<commit_message>
added device serial number lookup
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim_braly/ZTP-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdeterra\Documents\Customers\Hanscom AFB\ZTP Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="740" windowWidth="28800" windowHeight="16540"/>
+    <workbookView xWindow="1116" yWindow="744" windowWidth="28800" windowHeight="16536"/>
   </bookViews>
   <sheets>
     <sheet name="SWITCHES" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>snmp_location</t>
   </si>
@@ -101,9 +101,6 @@
     <t>e 1/1/45 to 1/1/48</t>
   </si>
   <si>
-    <t>10.0.0.222</t>
-  </si>
-  <si>
     <t>10.0.0.1</t>
   </si>
   <si>
@@ -114,12 +111,51 @@
   </si>
   <si>
     <t>e 1/1/3 to 1/1/44</t>
+  </si>
+  <si>
+    <t>10.0.0.2</t>
+  </si>
+  <si>
+    <t>10.0.0.3</t>
+  </si>
+  <si>
+    <t>e 1/1/3 to 1/1/6</t>
+  </si>
+  <si>
+    <t>e 1/1/7 to 1/1/12</t>
+  </si>
+  <si>
+    <t>ICX6450_template_A</t>
+  </si>
+  <si>
+    <t>10.0.0.20</t>
+  </si>
+  <si>
+    <t>00:06:cc:4e:24:c1_0/10/1/3</t>
+  </si>
+  <si>
+    <t>10.0.0.4</t>
+  </si>
+  <si>
+    <t>00:06:cc:4e:24:c1_0/10/1/5</t>
+  </si>
+  <si>
+    <t>ZTP_ICX6450_SW1</t>
+  </si>
+  <si>
+    <t>ZTP_ICX6450_SW2</t>
+  </si>
+  <si>
+    <t>CTG2549K09L</t>
+  </si>
+  <si>
+    <t>ZTP_ICX6450_SERIAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,6 +196,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -450,31 +489,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
+    <col min="7" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.6640625" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -500,7 +539,7 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -527,7 +566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -544,13 +583,13 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>10</v>
@@ -559,25 +598,184 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2">
         <v>201</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2">
         <v>1001</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P2">
         <v>2001</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3">
+        <v>201</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3">
+        <v>1001</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>2001</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>201</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4">
+        <v>1001</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>2001</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5">
+        <v>201</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5">
+        <v>1001</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>2001</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>